<commit_message>
(in progress) - Map similarly structured data from multiple workbooks/worksheets to a single 'Master' ListObject
</commit_message>
<xml_diff>
--- a/MatchMoveConsolidate/Inputsheet.xlsx
+++ b/MatchMoveConsolidate/Inputsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrower/projects/just-VBA/MatchMoveConsolidate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2464746-143D-C946-920D-69C53F0EF233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4C4D63-751C-3344-BB4A-75FB86D9AD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14200" yWindow="4960" windowWidth="34540" windowHeight="16440" activeTab="4" xr2:uid="{E4B1AFDB-9D25-DD46-A9DC-84EEF11C9041}"/>
+    <workbookView xWindow="23780" yWindow="13720" windowWidth="27220" windowHeight="15120" xr2:uid="{E4B1AFDB-9D25-DD46-A9DC-84EEF11C9041}"/>
   </bookViews>
   <sheets>
     <sheet name="CompanyA (1)" sheetId="1" r:id="rId1"/>
@@ -247,6 +247,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF941100"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -729,10 +734,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0205A0AA-F82F-4E46-9093-38489E3624D3}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1">
+    <tabColor rgb="FF941100"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1059,7 +1066,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FB172A-BE67-6D4B-AAE2-BC87A9A427F5}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2">
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1388,7 +1397,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E09553-B5A6-2A45-92B2-1FBF7E126171}">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3">
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
@@ -1718,7 +1729,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDAA7B8D-6C1C-2848-AC60-15674D4A0769}">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet4">
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1731,10 +1744,12 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCE493E-4C3B-BD40-9D72-8A9CC1F902D7}">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5">
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -2048,7 +2063,328 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF0BDD1-9677-2040-A738-25DC9A654D34}">
-  <sheetPr codeName="Sheet6"/>
+  <sheetPr codeName="Sheet6">
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="G1:R8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="7:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>44571</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44573</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2114.1999999999998</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2114.1999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <f>G2+1</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>44588</v>
+      </c>
+      <c r="I3" s="2">
+        <v>44588</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="1">
+        <v>531.64</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1582.56</v>
+      </c>
+    </row>
+    <row r="4" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="0">G3+1</f>
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>44589</v>
+      </c>
+      <c r="I4" s="2">
+        <v>44589</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="1">
+        <v>972.96</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" s="1">
+        <v>609.6</v>
+      </c>
+    </row>
+    <row r="5" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>44592</v>
+      </c>
+      <c r="I5" s="2">
+        <v>44592</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="1">
+        <v>214.69</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" s="1">
+        <v>394.91</v>
+      </c>
+    </row>
+    <row r="6" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>44605</v>
+      </c>
+      <c r="I6" s="2">
+        <v>44605</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1"/>
+      <c r="Q6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="2">
+        <v>44620</v>
+      </c>
+      <c r="I7" s="2">
+        <v>44620</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="7:18" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H8" s="2">
+        <v>44709</v>
+      </c>
+      <c r="I8" s="2">
+        <v>44709</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="1">
+        <v>394.91</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" s="1">
+        <v>394.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770DD188-51C8-4445-ACD7-D6EE39399CEA}">
+  <sheetPr codeName="Sheet7">
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2363,330 +2699,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770DD188-51C8-4445-ACD7-D6EE39399CEA}">
-  <sheetPr codeName="Sheet7"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC856D7-15E8-2544-9830-1F68D057DAE8}">
+  <sheetPr codeName="Sheet8">
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="G1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:R8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="7:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="G1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>44571</v>
-      </c>
-      <c r="I2" s="2">
-        <v>44573</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>2114.1999999999998</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="1">
-        <v>2114.1999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G3">
-        <f>G2+1</f>
-        <v>2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>44588</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44588</v>
-      </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O3" s="1">
-        <v>531.64</v>
-      </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1582.56</v>
-      </c>
-    </row>
-    <row r="4" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G4">
-        <f t="shared" ref="G4:G8" si="0">G3+1</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>44589</v>
-      </c>
-      <c r="I4" s="2">
-        <v>44589</v>
-      </c>
-      <c r="J4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O4" s="1">
-        <v>972.96</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="1">
-        <v>609.6</v>
-      </c>
-    </row>
-    <row r="5" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H5" s="2">
-        <v>44592</v>
-      </c>
-      <c r="I5" s="2">
-        <v>44592</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="1">
-        <v>214.69</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="1">
-        <v>394.91</v>
-      </c>
-    </row>
-    <row r="6" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>44605</v>
-      </c>
-      <c r="I6" s="2">
-        <v>44605</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O6" s="1">
-        <v>0</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H7" s="2">
-        <v>44620</v>
-      </c>
-      <c r="I7" s="2">
-        <v>44620</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="7:18" x14ac:dyDescent="0.2">
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H8" s="2">
-        <v>44709</v>
-      </c>
-      <c r="I8" s="2">
-        <v>44709</v>
-      </c>
-      <c r="J8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" t="s">
-        <v>26</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="1">
-        <v>394.91</v>
-      </c>
-      <c r="P8" s="1"/>
-      <c r="Q8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R8" s="1">
-        <v>394.91</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC856D7-15E8-2544-9830-1F68D057DAE8}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="G1:R8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:R8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>